<commit_message>
Added an additional line for ensuring the deletion of cookies in browser.py Filtered the Municipalities by ensuring a mutual minimal distance of 20 kilometers.
</commit_message>
<xml_diff>
--- a/Experiment/Coordinates.xlsx
+++ b/Experiment/Coordinates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e8df5c317597596/Documenten/Master/Information_Retrieval/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdare\PycharmProjects\Information-Retrieval---Selenium\Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C801960-241C-40AE-8D3C-2B55471B2494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71C768D-A334-4339-883E-042E3B67B9AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="593" xr2:uid="{2E2B948F-80FD-41A8-A50B-9CAD7A901E77}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>{"latitude": 52.3545828, "longitude": 4.7638762, "accuracy": 1}</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Rucphen</t>
   </si>
   <si>
-    <t>Kerkrade</t>
-  </si>
-  <si>
     <t>Neder-betuwe</t>
   </si>
   <si>
@@ -101,63 +98,36 @@
     <t>Reimerswaal</t>
   </si>
   <si>
-    <t>Tholen</t>
-  </si>
-  <si>
     <t>Rijssen-holten</t>
   </si>
   <si>
     <t>Tubbergen</t>
   </si>
   <si>
-    <t>Dinkelland</t>
-  </si>
-  <si>
     <t>Nederweerd</t>
   </si>
   <si>
-    <t>Asten</t>
-  </si>
-  <si>
     <t>Raalte</t>
   </si>
   <si>
     <t>Eersel</t>
   </si>
   <si>
-    <t>Someren</t>
-  </si>
-  <si>
-    <t>Leudal</t>
-  </si>
-  <si>
     <t>Percentage</t>
   </si>
   <si>
     <t>41.8</t>
   </si>
   <si>
-    <t>39.7</t>
-  </si>
-  <si>
     <t>39.5</t>
   </si>
   <si>
-    <t>35.2</t>
-  </si>
-  <si>
     <t>30.3</t>
   </si>
   <si>
     <t>26.0</t>
   </si>
   <si>
-    <t>24.5</t>
-  </si>
-  <si>
-    <t>24.4</t>
-  </si>
-  <si>
     <t>37.7</t>
   </si>
   <si>
@@ -191,12 +161,6 @@
     <t>Hellevoetsluis</t>
   </si>
   <si>
-    <t>Nissewaard</t>
-  </si>
-  <si>
-    <t>24.9</t>
-  </si>
-  <si>
     <t>Westland</t>
   </si>
   <si>
@@ -209,12 +173,6 @@
     <t>24.0</t>
   </si>
   <si>
-    <t>Velsen</t>
-  </si>
-  <si>
-    <t>21.0</t>
-  </si>
-  <si>
     <t>Almelo</t>
   </si>
   <si>
@@ -242,18 +200,12 @@
     <t>28.1</t>
   </si>
   <si>
-    <t>Gooise Meren</t>
-  </si>
-  <si>
     <t>{"latitude": 52.1410334, "longitude": 4.3034182, "accuracy": 1}</t>
   </si>
   <si>
     <t>{"latitude": 52.4151142, "longitude": 4.5523355, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 52.3107638, "longitude": 5.0515749, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 51.5598461, "longitude": 4.6242571, "accuracy": 1}</t>
   </si>
   <si>
@@ -272,45 +224,27 @@
     <t>{"latitude": 51.8504908, "longitude": 4.0557649, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 51.8472776, "longitude": 4.302814, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 51.9984418, "longitude": 4.1485715, "accuracy": 1}</t>
   </si>
   <si>
     <t>{"latitude": 52.3810687, "longitude": 4.5187475, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 52.4499973, "longitude": 4.5575291, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 52.3609531, "longitude": 6.5892449, "accuracy": 1}</t>
   </si>
   <si>
     <t>{"latitude": 52.4091256, "longitude": 6.7430093, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 52.3713547, "longitude": 6.7755242, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 51.2840894, "longitude": 5.6560837, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 51.3862271, "longitude": 5.714951, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 52.3908088, "longitude": 6.1964119, "accuracy": 1}</t>
   </si>
   <si>
     <t>{"latitude": 51.3503862, "longitude": 5.2373018, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 51.233891, "longitude": 5.7383804, "accuracy": 1}</t>
-  </si>
-  <si>
-    <t>{"latitude": 51.3659169, "longitude": 5.6344824, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 51.9213568, "longitude": 5.5121256, "accuracy": 1}</t>
   </si>
   <si>
@@ -320,9 +254,6 @@
     <t>{"latitude": 52.6515548, "longitude": 6.1214943, "accuracy": 1}</t>
   </si>
   <si>
-    <t>{"latitude": 51.537127, "longitude": 4.1227367, "accuracy": 1}</t>
-  </si>
-  <si>
     <t>{"latitude": 52.2843192, "longitude": 6.3700717, "accuracy": 1}</t>
   </si>
   <si>
@@ -330,9 +261,6 @@
   </si>
   <si>
     <t>{"latitude": 50.902539, "longitude": 5.9724238, "accuracy": 1}</t>
-  </si>
-  <si>
-    <t>{"latitude": 50.8682113, "longitude": 6.009308, "accuracy": 1}</t>
   </si>
 </sst>
 </file>
@@ -726,7 +654,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -759,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C2" s="3">
         <v>51.528890599999997</v>
@@ -768,7 +696,7 @@
         <v>4.5062265000000004</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -778,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C3" s="3">
         <v>50.902538999999997</v>
@@ -787,27 +715,14 @@
         <v>5.9724237999999996</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3">
-        <v>50.868211299999999</v>
-      </c>
-      <c r="D4" s="3">
-        <v>6.0093079999999999</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
@@ -822,7 +737,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -852,10 +767,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3">
         <v>51.921356799999998</v>
@@ -864,17 +779,17 @@
         <v>5.5121256000000001</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3">
         <v>51.507499099999997</v>
@@ -883,17 +798,17 @@
         <v>4.1637452000000001</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3">
         <v>52.6515548</v>
@@ -902,46 +817,31 @@
         <v>6.1214943000000002</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3">
-        <v>51.537126999999998</v>
+        <v>52.284319199999999</v>
       </c>
       <c r="D5" s="3">
-        <v>4.1227366999999999</v>
+        <v>6.3700716999999996</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3">
-        <v>52.284319199999999</v>
-      </c>
-      <c r="D6" s="3">
-        <v>6.3700716999999996</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
@@ -956,7 +856,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -986,10 +886,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>52.409125600000003</v>
@@ -998,141 +898,85 @@
         <v>6.7430092999999998</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3">
-        <v>52.371354699999998</v>
+        <v>51.284089399999999</v>
       </c>
       <c r="D3" s="3">
-        <v>6.7755242000000004</v>
+        <v>5.6560836999999999</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3">
-        <v>51.284089399999999</v>
+        <v>52.390808800000002</v>
       </c>
       <c r="D4" s="3">
-        <v>5.6560836999999999</v>
+        <v>6.1964119000000002</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3">
-        <v>51.386227099999999</v>
+        <v>51.350386200000003</v>
       </c>
       <c r="D5" s="3">
-        <v>5.7149510000000001</v>
+        <v>5.2373018</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="3">
-        <v>52.390808800000002</v>
-      </c>
-      <c r="D6" s="3">
-        <v>6.1964119000000002</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="3">
-        <v>51.350386200000003</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5.2373018</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="3">
-        <v>51.233891</v>
-      </c>
-      <c r="D8" s="3">
-        <v>5.7383803999999996</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3">
-        <v>51.365916900000002</v>
-      </c>
-      <c r="D9" s="3">
-        <v>5.6344823999999996</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
@@ -1144,10 +988,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{560078F0-0554-4AC1-907E-349181259D29}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -1177,10 +1021,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>52.500192599999998</v>
@@ -1189,15 +1033,15 @@
         <v>5.0403517999999998</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>51.850490800000003</v>
@@ -1206,92 +1050,58 @@
         <v>4.0557648999999998</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C4">
-        <v>51.847277599999998</v>
+        <v>51.998441800000002</v>
       </c>
       <c r="D4">
-        <v>4.3028139999999997</v>
+        <v>4.1485715000000001</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>51.998441800000002</v>
+        <v>52.3810687</v>
       </c>
       <c r="D5">
-        <v>4.1485715000000001</v>
+        <v>4.5187474999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>52.3810687</v>
+        <v>52.360953100000003</v>
       </c>
       <c r="D6">
-        <v>4.5187474999999999</v>
+        <v>6.5892448999999997</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7">
-        <v>52.4499973</v>
-      </c>
-      <c r="D7">
-        <v>4.5575291</v>
-      </c>
-      <c r="E7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8">
-        <v>52.360953100000003</v>
-      </c>
-      <c r="D8">
-        <v>6.5892448999999997</v>
-      </c>
-      <c r="E8" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1132,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -1339,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C2" s="10">
         <v>52.084166000000003</v>
@@ -1348,7 +1158,7 @@
         <v>5.0124515000000001</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1356,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C3" s="9">
         <v>52.354582800000003</v>
@@ -1373,7 +1183,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C4" s="9">
         <v>51.842841300000003</v>
@@ -1382,7 +1192,7 @@
         <v>5.7631167000000003</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1390,7 +1200,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C5" s="9">
         <v>53.221684500000002</v>
@@ -1399,7 +1209,7 @@
         <v>6.4956534000000001</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1223,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1429,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -1446,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C2" s="7">
         <v>52.242501900000001</v>
@@ -1464,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4">
         <v>52.141033399999998</v>
@@ -1473,7 +1283,7 @@
         <v>4.3034182000000003</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F3" s="3"/>
     </row>
@@ -1482,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3">
         <v>52.415114199999998</v>
@@ -1491,44 +1301,29 @@
         <v>4.5523354999999999</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3">
-        <v>52.310763799999997</v>
+        <v>51.559846100000001</v>
       </c>
       <c r="D5" s="3">
-        <v>5.0515749000000003</v>
+        <v>4.6242571000000003</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="3">
-        <v>51.559846100000001</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4.6242571000000003</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="F6" s="3"/>
     </row>
   </sheetData>

</xml_diff>